<commit_message>
Updated script and qa report
</commit_message>
<xml_diff>
--- a/Scripts/Input/Qualitative Analysis Report_all.xlsx
+++ b/Scripts/Input/Qualitative Analysis Report_all.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project GC-MS\GC-MS\Files - GCMS - Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project GC-MS\GC-MS\Scripts\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8032A628-32C4-42C9-BB8D-3CA4DF109F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47887650-D70C-4771-BB02-8A106A74975A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="7">
   <si>
     <t>Area °/a</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Area</t>
-  </si>
-  <si>
-    <t>.3.082</t>
   </si>
 </sst>
 </file>
@@ -983,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1027,8 +1024,8 @@
       <c r="B2" s="18">
         <v>3.069</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>7</v>
+      <c r="C2" s="10">
+        <v>3.0819999999999999</v>
       </c>
       <c r="D2" s="18">
         <v>3.2120000000000002</v>
@@ -2086,7 +2083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>

</xml_diff>